<commit_message>
probleme de chargement xlsx
</commit_message>
<xml_diff>
--- a/src/loader_package/pre_load.xlsx
+++ b/src/loader_package/pre_load.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ecole\ING3\Informatique\Projet\java_project_desautel_pellen_perold\src\loader_package\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128BFF5A-1BDB-4D89-8BDE-1F74250DE143}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EC927C-C23C-45ED-B119-CAF9A5183C34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="elector" sheetId="1" r:id="rId1"/>
@@ -29,40 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>nameState</t>
-  </si>
-  <si>
-    <t>lastnameCandidat</t>
-  </si>
-  <si>
-    <t>party</t>
-  </si>
-  <si>
-    <t>nbrVoteTotal</t>
-  </si>
-  <si>
-    <t>vote</t>
-  </si>
-  <si>
-    <t>allWins</t>
-  </si>
-  <si>
-    <t>nbrMaxElectors</t>
-  </si>
-  <si>
-    <t>pause</t>
-  </si>
-  <si>
-    <t>openVote</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Perold</t>
   </si>
@@ -76,9 +43,6 @@
     <t>Biden</t>
   </si>
   <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>Joe</t>
   </si>
   <si>
@@ -121,7 +85,31 @@
     <t>Junior</t>
   </si>
   <si>
-    <t>true</t>
+    <t>password</t>
+  </si>
+  <si>
+    <t>password1</t>
+  </si>
+  <si>
+    <t>loser</t>
+  </si>
+  <si>
+    <t>cœur</t>
+  </si>
+  <si>
+    <t>14/18</t>
+  </si>
+  <si>
+    <t>seatibiza</t>
+  </si>
+  <si>
+    <t>Toko</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>lokopoto</t>
   </si>
 </sst>
 </file>
@@ -178,11 +166,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -478,106 +463,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.21875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="F3" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="6" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E10" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -587,59 +584,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCABBEE2-3395-47C2-9626-C3684E3ED960}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="E1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3">
+      <c r="E2">
         <v>1</v>
       </c>
     </row>
@@ -652,79 +641,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1851D91F-DA7C-4EA5-959B-DCDBAE8FBF58}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B3">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
       <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D5" s="3"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D6" s="3"/>
+      <c r="D6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -736,7 +711,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,29 +721,25 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -777,10 +748,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{883CD6C9-C7F8-417C-AF0A-CD6526D333C3}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -788,14 +759,9 @@
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>30</v>
+    <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version de sauvegarde (non opérationnelle)
Réglage du problème : trop de connexions
</commit_message>
<xml_diff>
--- a/src/loader_package/pre_load.xlsx
+++ b/src/loader_package/pre_load.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ecole\ING3\Informatique\Projet\java_project_desautel_pellen_perold\src\loader_package\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\java_project_desautel_pellen_perold\src\loader_package\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EC927C-C23C-45ED-B119-CAF9A5183C34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604A0AF3-4582-4EAF-84AF-48C2017A1864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="elector" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Perold</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>Repu</t>
-  </si>
-  <si>
-    <t>Wadhington</t>
   </si>
   <si>
     <t>Fercoq</t>
@@ -466,19 +463,19 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.21875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -486,7 +483,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
@@ -498,7 +495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -506,7 +503,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>8</v>
@@ -518,7 +515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -526,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>11</v>
@@ -538,15 +535,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>11</v>
@@ -558,22 +555,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E10" s="4"/>
     </row>
   </sheetData>
@@ -590,15 +587,15 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -606,7 +603,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
@@ -615,7 +612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -623,7 +620,7 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -642,18 +639,18 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -667,9 +664,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>15</v>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -681,7 +678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -695,10 +692,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
     </row>
   </sheetData>
@@ -714,30 +711,30 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
@@ -754,12 +751,12 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
All candidates + choix start / pause / end vote fait
</commit_message>
<xml_diff>
--- a/src/loader_package/pre_load.xlsx
+++ b/src/loader_package/pre_load.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\java_project_desautel_pellen_perold\src\loader_package\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://poce-my.sharepoint.com/personal/charles_perold_edu_ece_fr/Documents/ING 3/Informatique - Java/_Projet Gui S5/_Projet GUI_Fork/java_project_desautel_pellen_perold/src/loader_package/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604A0AF3-4582-4EAF-84AF-48C2017A1864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{604A0AF3-4582-4EAF-84AF-48C2017A1864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ADD78C17-4C26-47EF-8109-2C63ED9F4FDD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4166" yWindow="2520" windowWidth="22680" windowHeight="11443" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="elector" sheetId="1" r:id="rId1"/>
@@ -163,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -179,6 +179,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,20 +465,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8.3828125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.69140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.69140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.69140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.3046875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -495,7 +498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -515,7 +518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -535,7 +538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -555,22 +558,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E10" s="4"/>
     </row>
   </sheetData>
@@ -583,19 +586,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCABBEE2-3395-47C2-9626-C3684E3ED960}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -612,17 +615,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E2">
@@ -642,15 +645,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -664,7 +667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -678,7 +681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -692,10 +695,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="D6" s="2"/>
     </row>
   </sheetData>
@@ -711,12 +714,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -727,14 +730,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.9" x14ac:dyDescent="0.4">
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
@@ -751,12 +754,12 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A1" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Mise à jour excel
</commit_message>
<xml_diff>
--- a/src/loader_package/pre_load.xlsx
+++ b/src/loader_package/pre_load.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://poce-my.sharepoint.com/personal/charles_perold_edu_ece_fr/Documents/ING 3/Informatique - Java/_Projet Gui S5/_Projet GUI_Fork/java_project_desautel_pellen_perold/src/loader_package/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\java_project_desautel_pellen_perold\src\loader_package\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{604A0AF3-4582-4EAF-84AF-48C2017A1864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ADD78C17-4C26-47EF-8109-2C63ED9F4FDD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604A0AF3-4582-4EAF-84AF-48C2017A1864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4166" yWindow="2520" windowWidth="22680" windowHeight="11443" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="elector" sheetId="1" r:id="rId1"/>
@@ -163,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -179,9 +179,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -465,20 +462,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.3828125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.69140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.69140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.69140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.3046875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -498,7 +495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -518,7 +515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -538,7 +535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -558,22 +555,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E10" s="4"/>
     </row>
   </sheetData>
@@ -586,19 +583,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCABBEE2-3395-47C2-9626-C3684E3ED960}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.3828125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.69140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -615,17 +612,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
       <c r="E2">
@@ -645,15 +642,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -667,7 +664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -681,7 +678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -695,10 +692,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
     </row>
   </sheetData>
@@ -714,12 +711,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -730,14 +727,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
@@ -754,12 +751,12 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
UltimateDrivingMachine by BMW M Performance
</commit_message>
<xml_diff>
--- a/src/loader_package/pre_load.xlsx
+++ b/src/loader_package/pre_load.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\java_project_desautel_pellen_perold\src\loader_package\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://poce-my.sharepoint.com/personal/charles_perold_edu_ece_fr/Documents/ING 3/Informatique - Java/_Projet Gui S5/_Projet GUI_Fork/java_project_desautel_pellen_perold/src/loader_package/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604A0AF3-4582-4EAF-84AF-48C2017A1864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{604A0AF3-4582-4EAF-84AF-48C2017A1864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{902BB13C-8636-4D3C-8729-209E0745611E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3823" yWindow="2177" windowWidth="22680" windowHeight="11443" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="elector" sheetId="1" r:id="rId1"/>
@@ -97,9 +97,6 @@
     <t>14/18</t>
   </si>
   <si>
-    <t>seatibiza</t>
-  </si>
-  <si>
     <t>Toko</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
   </si>
   <si>
     <t>lokopoto</t>
+  </si>
+  <si>
+    <t>DrivingMachine</t>
   </si>
 </sst>
 </file>
@@ -163,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -179,6 +179,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,27 +466,27 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8.3828125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.69140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.69140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.69140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.3046875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>22</v>
+      <c r="C1" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
@@ -495,14 +498,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -515,14 +518,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -535,15 +538,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>11</v>
@@ -555,22 +558,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C5" s="6"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="E10" s="4"/>
     </row>
   </sheetData>
@@ -587,15 +591,15 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -612,7 +616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -642,15 +646,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -664,7 +668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -678,7 +682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -692,10 +696,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="D6" s="2"/>
     </row>
   </sheetData>
@@ -711,12 +715,12 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -727,14 +731,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.9" x14ac:dyDescent="0.4">
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
@@ -751,12 +755,12 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A1" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Fonctions : Add Candidate / Del Candidate / Add Elector (bug) / Dell Elector / Affichage intelligent des candidats
</commit_message>
<xml_diff>
--- a/src/loader_package/pre_load.xlsx
+++ b/src/loader_package/pre_load.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://poce-my.sharepoint.com/personal/charles_perold_edu_ece_fr/Documents/ING 3/Informatique - Java/_Projet Gui S5/_Projet GUI_Fork/java_project_desautel_pellen_perold/src/loader_package/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{604A0AF3-4582-4EAF-84AF-48C2017A1864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{902BB13C-8636-4D3C-8729-209E0745611E}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{604A0AF3-4582-4EAF-84AF-48C2017A1864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E00CE3EB-4B32-4836-ADFC-E53526E7DD3E}"/>
   <bookViews>
-    <workbookView xWindow="3823" yWindow="2177" windowWidth="22680" windowHeight="11443" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="27977" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="elector" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Perold</t>
   </si>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t>DrivingMachine</t>
+  </si>
+  <si>
+    <t>Lefou</t>
+  </si>
+  <si>
+    <t>Oupas</t>
+  </si>
+  <si>
+    <t>tg</t>
+  </si>
+  <si>
+    <t>jesaispas</t>
   </si>
 </sst>
 </file>
@@ -465,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -585,10 +597,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCABBEE2-3395-47C2-9626-C3684E3ED960}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -631,6 +643,23 @@
       </c>
       <c r="E2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>